<commit_message>
feat: add script to generate context diagram from session data
This commit introduces a new script that reads session data from a CSV file, processes it using the Gemini API, and generates a markdown file summarizing the technical trends and their applications. The script is designed to create a structured context diagram for better understanding and visualization of the trends discussed in the sessions.
</commit_message>
<xml_diff>
--- a/google_next_sessions.xlsx
+++ b/google_next_sessions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfh00896102/Github/google_next/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A99E354-0D9D-9944-A839-6E2E93ADE792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4689773-3519-AB4D-9189-0D160210ADF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6255,11 +6255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -6287,7 +6286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6298,7 +6297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -6309,7 +6308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -6320,7 +6319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -6331,7 +6330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -6348,7 +6347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -6399,7 +6398,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -6416,7 +6415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -6450,7 +6449,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -6461,7 +6460,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -6495,7 +6494,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -6512,7 +6511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -6529,7 +6528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -6546,7 +6545,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -6563,7 +6562,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -6580,7 +6579,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -6597,7 +6596,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -6608,7 +6607,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -6642,7 +6641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -6659,7 +6658,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -6670,7 +6669,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -6681,7 +6680,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -6698,7 +6697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -6732,7 +6731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -6749,7 +6748,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>126</v>
       </c>
@@ -6760,7 +6759,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -6771,7 +6770,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -6788,7 +6787,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -6805,7 +6804,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -6833,7 +6832,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -6844,7 +6843,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -6855,7 +6854,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -6872,7 +6871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>157</v>
       </c>
@@ -6889,7 +6888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -6906,7 +6905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -6917,7 +6916,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>168</v>
       </c>
@@ -6934,7 +6933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>172</v>
       </c>
@@ -6968,7 +6967,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>180</v>
       </c>
@@ -6985,7 +6984,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>185</v>
       </c>
@@ -6996,7 +6995,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>188</v>
       </c>
@@ -7013,7 +7012,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>192</v>
       </c>
@@ -7030,7 +7029,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -7047,7 +7046,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>200</v>
       </c>
@@ -7064,7 +7063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>204</v>
       </c>
@@ -7081,7 +7080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>208</v>
       </c>
@@ -7098,7 +7097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>212</v>
       </c>
@@ -7115,7 +7114,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>216</v>
       </c>
@@ -7132,7 +7131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>220</v>
       </c>
@@ -7149,7 +7148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -7160,7 +7159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -7171,7 +7170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>224</v>
       </c>
@@ -7188,7 +7187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>228</v>
       </c>
@@ -7199,7 +7198,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>231</v>
       </c>
@@ -7210,7 +7209,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>234</v>
       </c>
@@ -7221,7 +7220,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>237</v>
       </c>
@@ -7232,7 +7231,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>240</v>
       </c>
@@ -7243,7 +7242,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>243</v>
       </c>
@@ -7260,7 +7259,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>247</v>
       </c>
@@ -7277,7 +7276,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>251</v>
       </c>
@@ -7294,7 +7293,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>255</v>
       </c>
@@ -7311,7 +7310,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>260</v>
       </c>
@@ -7328,7 +7327,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>264</v>
       </c>
@@ -7345,7 +7344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>268</v>
       </c>
@@ -7362,7 +7361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>272</v>
       </c>
@@ -7379,7 +7378,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>276</v>
       </c>
@@ -7396,7 +7395,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>280</v>
       </c>
@@ -7413,7 +7412,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>284</v>
       </c>
@@ -7424,7 +7423,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>287</v>
       </c>
@@ -7441,7 +7440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>291</v>
       </c>
@@ -7458,7 +7457,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>295</v>
       </c>
@@ -7475,7 +7474,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>299</v>
       </c>
@@ -7492,7 +7491,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>304</v>
       </c>
@@ -7509,7 +7508,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>309</v>
       </c>
@@ -7526,7 +7525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>313</v>
       </c>
@@ -7543,7 +7542,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>317</v>
       </c>
@@ -7560,7 +7559,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>321</v>
       </c>
@@ -7577,7 +7576,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>325</v>
       </c>
@@ -7588,7 +7587,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>328</v>
       </c>
@@ -7599,7 +7598,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="30" hidden="1">
+    <row r="88" spans="1:5" ht="30">
       <c r="A88" t="s">
         <v>1535</v>
       </c>
@@ -7616,7 +7615,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>334</v>
       </c>
@@ -7627,7 +7626,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>337</v>
       </c>
@@ -7644,7 +7643,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>341</v>
       </c>
@@ -7661,7 +7660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>345</v>
       </c>
@@ -7678,7 +7677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>349</v>
       </c>
@@ -7695,7 +7694,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>353</v>
       </c>
@@ -7712,7 +7711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>357</v>
       </c>
@@ -7729,7 +7728,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>361</v>
       </c>
@@ -7746,7 +7745,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>365</v>
       </c>
@@ -7757,7 +7756,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>368</v>
       </c>
@@ -7791,7 +7790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>376</v>
       </c>
@@ -7802,7 +7801,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>379</v>
       </c>
@@ -7819,7 +7818,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>383</v>
       </c>
@@ -7836,7 +7835,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>387</v>
       </c>
@@ -7847,7 +7846,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>390</v>
       </c>
@@ -7864,7 +7863,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>394</v>
       </c>
@@ -7881,7 +7880,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>399</v>
       </c>
@@ -7898,7 +7897,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>403</v>
       </c>
@@ -7915,7 +7914,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>407</v>
       </c>
@@ -7932,7 +7931,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>411</v>
       </c>
@@ -7943,7 +7942,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>414</v>
       </c>
@@ -7960,7 +7959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>418</v>
       </c>
@@ -7971,7 +7970,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>421</v>
       </c>
@@ -7988,7 +7987,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>425</v>
       </c>
@@ -8005,7 +8004,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>429</v>
       </c>
@@ -8022,7 +8021,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>434</v>
       </c>
@@ -8033,7 +8032,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>437</v>
       </c>
@@ -8044,7 +8043,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>440</v>
       </c>
@@ -8055,7 +8054,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>443</v>
       </c>
@@ -8072,7 +8071,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>447</v>
       </c>
@@ -8083,7 +8082,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>450</v>
       </c>
@@ -8100,7 +8099,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>455</v>
       </c>
@@ -8117,7 +8116,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>459</v>
       </c>
@@ -8134,7 +8133,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>464</v>
       </c>
@@ -8151,7 +8150,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>468</v>
       </c>
@@ -8168,7 +8167,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>472</v>
       </c>
@@ -8185,7 +8184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>476</v>
       </c>
@@ -8196,7 +8195,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>479</v>
       </c>
@@ -8207,7 +8206,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>482</v>
       </c>
@@ -8224,7 +8223,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>486</v>
       </c>
@@ -8241,7 +8240,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>490</v>
       </c>
@@ -8252,7 +8251,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
         <v>493</v>
       </c>
@@ -8269,7 +8268,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="30" hidden="1">
+    <row r="132" spans="1:5" ht="30">
       <c r="A132" t="s">
         <v>498</v>
       </c>
@@ -8286,7 +8285,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
         <v>502</v>
       </c>
@@ -8303,7 +8302,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
         <v>506</v>
       </c>
@@ -8320,7 +8319,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -8331,7 +8330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
         <v>14</v>
       </c>
@@ -8342,7 +8341,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
         <v>17</v>
       </c>
@@ -8353,7 +8352,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>510</v>
       </c>
@@ -8370,7 +8369,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
         <v>514</v>
       </c>
@@ -8387,7 +8386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
         <v>518</v>
       </c>
@@ -8398,7 +8397,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
         <v>521</v>
       </c>
@@ -8432,7 +8431,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>529</v>
       </c>
@@ -8443,7 +8442,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1">
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
         <v>532</v>
       </c>
@@ -8460,7 +8459,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
         <v>536</v>
       </c>
@@ -8471,7 +8470,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
         <v>539</v>
       </c>
@@ -8488,7 +8487,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
         <v>543</v>
       </c>
@@ -8505,7 +8504,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
         <v>547</v>
       </c>
@@ -8516,7 +8515,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
         <v>550</v>
       </c>
@@ -8533,7 +8532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
         <v>554</v>
       </c>
@@ -8550,7 +8549,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
         <v>558</v>
       </c>
@@ -8567,7 +8566,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
         <v>562</v>
       </c>
@@ -8584,7 +8583,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
         <v>566</v>
       </c>
@@ -8601,7 +8600,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
         <v>570</v>
       </c>
@@ -8618,7 +8617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
         <v>574</v>
       </c>
@@ -8635,7 +8634,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
+    <row r="156" spans="1:5">
       <c r="A156" t="s">
         <v>578</v>
       </c>
@@ -8652,7 +8651,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
+    <row r="157" spans="1:5">
       <c r="A157" t="s">
         <v>583</v>
       </c>
@@ -8669,7 +8668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1">
+    <row r="158" spans="1:5">
       <c r="A158" t="s">
         <v>587</v>
       </c>
@@ -8686,7 +8685,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1">
+    <row r="159" spans="1:5">
       <c r="A159" t="s">
         <v>591</v>
       </c>
@@ -8703,7 +8702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1">
+    <row r="160" spans="1:5">
       <c r="A160" t="s">
         <v>595</v>
       </c>
@@ -8720,7 +8719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1">
+    <row r="161" spans="1:5">
       <c r="A161" t="s">
         <v>599</v>
       </c>
@@ -8731,7 +8730,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1">
+    <row r="162" spans="1:5">
       <c r="A162" t="s">
         <v>602</v>
       </c>
@@ -8748,7 +8747,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1">
+    <row r="163" spans="1:5">
       <c r="A163" t="s">
         <v>606</v>
       </c>
@@ -8765,7 +8764,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1">
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
         <v>610</v>
       </c>
@@ -8782,7 +8781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1">
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
         <v>614</v>
       </c>
@@ -8799,7 +8798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1">
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
         <v>618</v>
       </c>
@@ -8816,7 +8815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1">
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
         <v>622</v>
       </c>
@@ -8833,7 +8832,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1">
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
         <v>626</v>
       </c>
@@ -8850,7 +8849,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1">
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
         <v>630</v>
       </c>
@@ -8884,7 +8883,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1">
+    <row r="171" spans="1:5">
       <c r="A171" t="s">
         <v>1537</v>
       </c>
@@ -8901,7 +8900,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:5" hidden="1">
+    <row r="172" spans="1:5">
       <c r="A172" t="s">
         <v>641</v>
       </c>
@@ -8918,7 +8917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1">
+    <row r="173" spans="1:5">
       <c r="A173" t="s">
         <v>645</v>
       </c>
@@ -8935,7 +8934,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1">
+    <row r="174" spans="1:5">
       <c r="A174" t="s">
         <v>649</v>
       </c>
@@ -8952,7 +8951,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="175" spans="1:5" hidden="1">
+    <row r="175" spans="1:5">
       <c r="A175" t="s">
         <v>653</v>
       </c>
@@ -8969,7 +8968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1">
+    <row r="176" spans="1:5">
       <c r="A176" t="s">
         <v>657</v>
       </c>
@@ -9003,7 +9002,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:5" hidden="1">
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
         <v>665</v>
       </c>
@@ -9014,7 +9013,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1">
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
         <v>668</v>
       </c>
@@ -9031,7 +9030,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1">
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
         <v>672</v>
       </c>
@@ -9048,7 +9047,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1">
+    <row r="181" spans="1:5">
       <c r="A181" t="s">
         <v>677</v>
       </c>
@@ -9065,7 +9064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1">
+    <row r="182" spans="1:5">
       <c r="A182" t="s">
         <v>681</v>
       </c>
@@ -9082,7 +9081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1">
+    <row r="183" spans="1:5">
       <c r="A183" t="s">
         <v>685</v>
       </c>
@@ -9093,7 +9092,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1">
+    <row r="184" spans="1:5">
       <c r="A184" t="s">
         <v>688</v>
       </c>
@@ -9110,7 +9109,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1">
+    <row r="185" spans="1:5">
       <c r="A185" t="s">
         <v>692</v>
       </c>
@@ -9127,7 +9126,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1">
+    <row r="186" spans="1:5">
       <c r="A186" t="s">
         <v>696</v>
       </c>
@@ -9161,7 +9160,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1">
+    <row r="188" spans="1:5">
       <c r="A188" t="s">
         <v>22</v>
       </c>
@@ -9172,7 +9171,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1">
+    <row r="189" spans="1:5">
       <c r="A189" t="s">
         <v>704</v>
       </c>
@@ -9189,7 +9188,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1">
+    <row r="190" spans="1:5">
       <c r="A190" t="s">
         <v>708</v>
       </c>
@@ -9200,7 +9199,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1">
+    <row r="191" spans="1:5">
       <c r="A191" t="s">
         <v>711</v>
       </c>
@@ -9217,7 +9216,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="192" spans="1:5" hidden="1">
+    <row r="192" spans="1:5">
       <c r="A192" t="s">
         <v>715</v>
       </c>
@@ -9234,7 +9233,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1">
+    <row r="193" spans="1:5">
       <c r="A193" t="s">
         <v>719</v>
       </c>
@@ -9251,7 +9250,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1">
+    <row r="194" spans="1:5">
       <c r="A194" t="s">
         <v>723</v>
       </c>
@@ -9268,7 +9267,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
         <v>727</v>
       </c>
@@ -9285,7 +9284,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1">
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
         <v>731</v>
       </c>
@@ -9296,7 +9295,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1">
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
         <v>734</v>
       </c>
@@ -9313,7 +9312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1">
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
         <v>738</v>
       </c>
@@ -9330,7 +9329,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1">
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
         <v>742</v>
       </c>
@@ -9347,7 +9346,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1">
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
         <v>746</v>
       </c>
@@ -9375,7 +9374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1">
+    <row r="202" spans="1:5">
       <c r="A202" t="s">
         <v>753</v>
       </c>
@@ -9392,7 +9391,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1">
+    <row r="203" spans="1:5">
       <c r="A203" t="s">
         <v>757</v>
       </c>
@@ -9409,7 +9408,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1">
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
         <v>761</v>
       </c>
@@ -9426,7 +9425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1">
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
         <v>765</v>
       </c>
@@ -9443,7 +9442,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1">
+    <row r="206" spans="1:5">
       <c r="A206" t="s">
         <v>769</v>
       </c>
@@ -9460,7 +9459,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1">
+    <row r="207" spans="1:5">
       <c r="A207" t="s">
         <v>773</v>
       </c>
@@ -9477,7 +9476,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="30" hidden="1">
+    <row r="208" spans="1:5" ht="30">
       <c r="A208" t="s">
         <v>777</v>
       </c>
@@ -9494,7 +9493,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1">
+    <row r="209" spans="1:5">
       <c r="A209" t="s">
         <v>781</v>
       </c>
@@ -9511,7 +9510,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
         <v>785</v>
       </c>
@@ -9528,7 +9527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1">
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
         <v>789</v>
       </c>
@@ -9545,7 +9544,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1">
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
         <v>793</v>
       </c>
@@ -9562,7 +9561,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1">
+    <row r="213" spans="1:5">
       <c r="A213" t="s">
         <v>797</v>
       </c>
@@ -9579,7 +9578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1">
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
         <v>801</v>
       </c>
@@ -9590,7 +9589,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1">
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
         <v>804</v>
       </c>
@@ -9607,7 +9606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1">
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>808</v>
       </c>
@@ -9624,7 +9623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="1:5" hidden="1">
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>812</v>
       </c>
@@ -9641,7 +9640,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1">
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
         <v>816</v>
       </c>
@@ -9652,7 +9651,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>819</v>
       </c>
@@ -9669,7 +9668,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
         <v>823</v>
       </c>
@@ -9686,7 +9685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1">
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>827</v>
       </c>
@@ -9697,7 +9696,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1">
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
         <v>830</v>
       </c>
@@ -9731,7 +9730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1">
+    <row r="224" spans="1:5">
       <c r="A224" t="s">
         <v>838</v>
       </c>
@@ -9742,7 +9741,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1">
+    <row r="225" spans="1:5">
       <c r="A225" t="s">
         <v>841</v>
       </c>
@@ -9759,7 +9758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1">
+    <row r="226" spans="1:5">
       <c r="A226" t="s">
         <v>845</v>
       </c>
@@ -9776,7 +9775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1">
+    <row r="227" spans="1:5">
       <c r="A227" t="s">
         <v>849</v>
       </c>
@@ -9793,7 +9792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1">
+    <row r="228" spans="1:5">
       <c r="A228" t="s">
         <v>853</v>
       </c>
@@ -9804,7 +9803,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1">
+    <row r="229" spans="1:5">
       <c r="A229" t="s">
         <v>856</v>
       </c>
@@ -9815,7 +9814,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1">
+    <row r="230" spans="1:5">
       <c r="A230" t="s">
         <v>859</v>
       </c>
@@ -9832,7 +9831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1">
+    <row r="231" spans="1:5">
       <c r="A231" t="s">
         <v>863</v>
       </c>
@@ -9849,7 +9848,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1">
+    <row r="232" spans="1:5">
       <c r="A232" t="s">
         <v>867</v>
       </c>
@@ -9866,7 +9865,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1">
+    <row r="233" spans="1:5">
       <c r="A233" t="s">
         <v>871</v>
       </c>
@@ -9877,7 +9876,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1">
+    <row r="234" spans="1:5">
       <c r="A234" t="s">
         <v>874</v>
       </c>
@@ -9894,7 +9893,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1">
+    <row r="235" spans="1:5">
       <c r="A235" t="s">
         <v>878</v>
       </c>
@@ -9905,7 +9904,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1">
+    <row r="236" spans="1:5">
       <c r="A236" t="s">
         <v>881</v>
       </c>
@@ -9922,7 +9921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1">
+    <row r="237" spans="1:5">
       <c r="A237" t="s">
         <v>885</v>
       </c>
@@ -9939,7 +9938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1">
+    <row r="238" spans="1:5">
       <c r="A238" t="s">
         <v>889</v>
       </c>
@@ -9956,7 +9955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1">
+    <row r="239" spans="1:5">
       <c r="A239" t="s">
         <v>893</v>
       </c>
@@ -9967,7 +9966,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1">
+    <row r="240" spans="1:5">
       <c r="A240" t="s">
         <v>896</v>
       </c>
@@ -9984,7 +9983,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
         <v>900</v>
       </c>
@@ -10001,7 +10000,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>904</v>
       </c>
@@ -10018,7 +10017,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1">
+    <row r="243" spans="1:5">
       <c r="A243" t="s">
         <v>908</v>
       </c>
@@ -10035,7 +10034,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1">
+    <row r="244" spans="1:5">
       <c r="A244" t="s">
         <v>912</v>
       </c>
@@ -10052,7 +10051,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1">
+    <row r="245" spans="1:5">
       <c r="A245" t="s">
         <v>916</v>
       </c>
@@ -10069,7 +10068,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="246" spans="1:5" hidden="1">
+    <row r="246" spans="1:5">
       <c r="A246" t="s">
         <v>920</v>
       </c>
@@ -10086,7 +10085,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="247" spans="1:5" hidden="1">
+    <row r="247" spans="1:5">
       <c r="A247" t="s">
         <v>924</v>
       </c>
@@ -10120,7 +10119,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="249" spans="1:5" hidden="1">
+    <row r="249" spans="1:5">
       <c r="A249" t="s">
         <v>932</v>
       </c>
@@ -10137,7 +10136,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1">
+    <row r="250" spans="1:5">
       <c r="A250" t="s">
         <v>936</v>
       </c>
@@ -10148,7 +10147,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="251" spans="1:5" hidden="1">
+    <row r="251" spans="1:5">
       <c r="A251" t="s">
         <v>939</v>
       </c>
@@ -10165,7 +10164,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="252" spans="1:5" hidden="1">
+    <row r="252" spans="1:5">
       <c r="A252" t="s">
         <v>26</v>
       </c>
@@ -10176,7 +10175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1">
+    <row r="253" spans="1:5">
       <c r="A253" t="s">
         <v>31</v>
       </c>
@@ -10187,7 +10186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="254" spans="1:5" hidden="1">
+    <row r="254" spans="1:5">
       <c r="A254" t="s">
         <v>943</v>
       </c>
@@ -10221,7 +10220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="256" spans="1:5" hidden="1">
+    <row r="256" spans="1:5">
       <c r="A256" t="s">
         <v>951</v>
       </c>
@@ -10238,7 +10237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
         <v>955</v>
       </c>
@@ -10255,7 +10254,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>35</v>
       </c>
@@ -10266,7 +10265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>959</v>
       </c>
@@ -10283,7 +10282,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>963</v>
       </c>
@@ -10300,7 +10299,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>967</v>
       </c>
@@ -10317,7 +10316,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>971</v>
       </c>
@@ -10334,7 +10333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="263" spans="1:5" hidden="1">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
         <v>975</v>
       </c>
@@ -10351,7 +10350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="264" spans="1:5" hidden="1">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
         <v>979</v>
       </c>
@@ -10368,7 +10367,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>983</v>
       </c>
@@ -10385,7 +10384,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1">
+    <row r="266" spans="1:5">
       <c r="A266" t="s">
         <v>987</v>
       </c>
@@ -10402,7 +10401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1">
+    <row r="267" spans="1:5">
       <c r="A267" t="s">
         <v>991</v>
       </c>
@@ -10419,7 +10418,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>995</v>
       </c>
@@ -10436,7 +10435,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1">
+    <row r="269" spans="1:5">
       <c r="A269" t="s">
         <v>999</v>
       </c>
@@ -10453,7 +10452,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1">
+    <row r="270" spans="1:5">
       <c r="A270" t="s">
         <v>1003</v>
       </c>
@@ -10470,7 +10469,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="271" spans="1:5" hidden="1">
+    <row r="271" spans="1:5">
       <c r="A271" t="s">
         <v>1007</v>
       </c>
@@ -10481,7 +10480,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="272" spans="1:5" hidden="1">
+    <row r="272" spans="1:5">
       <c r="A272" t="s">
         <v>1010</v>
       </c>
@@ -10498,7 +10497,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
         <v>1014</v>
       </c>
@@ -10515,7 +10514,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1">
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
         <v>1018</v>
       </c>
@@ -10532,7 +10531,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="275" spans="1:5" hidden="1">
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>1022</v>
       </c>
@@ -10549,7 +10548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="276" spans="1:5" hidden="1">
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>1026</v>
       </c>
@@ -10566,7 +10565,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="277" spans="1:5" hidden="1">
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>1030</v>
       </c>
@@ -10577,7 +10576,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1">
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>1033</v>
       </c>
@@ -10605,7 +10604,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1">
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>1040</v>
       </c>
@@ -10622,7 +10621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1">
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
         <v>1044</v>
       </c>
@@ -10639,7 +10638,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1">
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
         <v>1048</v>
       </c>
@@ -10656,7 +10655,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1">
+    <row r="283" spans="1:5">
       <c r="A283" t="s">
         <v>1052</v>
       </c>
@@ -10673,7 +10672,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1">
+    <row r="284" spans="1:5">
       <c r="A284" t="s">
         <v>1056</v>
       </c>
@@ -10690,7 +10689,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1">
+    <row r="285" spans="1:5">
       <c r="A285" t="s">
         <v>1060</v>
       </c>
@@ -10707,7 +10706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="30" hidden="1">
+    <row r="286" spans="1:5" ht="30">
       <c r="A286" t="s">
         <v>1064</v>
       </c>
@@ -10724,7 +10723,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1">
+    <row r="287" spans="1:5">
       <c r="A287" t="s">
         <v>1068</v>
       </c>
@@ -10741,7 +10740,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1">
+    <row r="288" spans="1:5">
       <c r="A288" t="s">
         <v>1072</v>
       </c>
@@ -10758,7 +10757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="289" spans="1:5" hidden="1">
+    <row r="289" spans="1:5">
       <c r="A289" t="s">
         <v>1076</v>
       </c>
@@ -10775,7 +10774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="290" spans="1:5" hidden="1">
+    <row r="290" spans="1:5">
       <c r="A290" t="s">
         <v>1080</v>
       </c>
@@ -10792,7 +10791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="291" spans="1:5" hidden="1">
+    <row r="291" spans="1:5">
       <c r="A291" t="s">
         <v>1084</v>
       </c>
@@ -10809,7 +10808,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1">
+    <row r="292" spans="1:5">
       <c r="A292" t="s">
         <v>1088</v>
       </c>
@@ -10826,7 +10825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1">
+    <row r="293" spans="1:5">
       <c r="A293" t="s">
         <v>1092</v>
       </c>
@@ -10843,7 +10842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1">
+    <row r="294" spans="1:5">
       <c r="A294" t="s">
         <v>1096</v>
       </c>
@@ -10860,7 +10859,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="295" spans="1:5" hidden="1">
+    <row r="295" spans="1:5">
       <c r="A295" t="s">
         <v>1100</v>
       </c>
@@ -10877,7 +10876,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1">
+    <row r="296" spans="1:5">
       <c r="A296" t="s">
         <v>1104</v>
       </c>
@@ -10894,7 +10893,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="297" spans="1:5" hidden="1">
+    <row r="297" spans="1:5">
       <c r="A297" t="s">
         <v>1108</v>
       </c>
@@ -10911,7 +10910,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1">
+    <row r="298" spans="1:5">
       <c r="A298" t="s">
         <v>1112</v>
       </c>
@@ -10928,7 +10927,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="299" spans="1:5" hidden="1">
+    <row r="299" spans="1:5">
       <c r="A299" t="s">
         <v>1116</v>
       </c>
@@ -10945,7 +10944,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1">
+    <row r="300" spans="1:5">
       <c r="A300" t="s">
         <v>1120</v>
       </c>
@@ -10956,7 +10955,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="301" spans="1:5" hidden="1">
+    <row r="301" spans="1:5">
       <c r="A301" t="s">
         <v>1123</v>
       </c>
@@ -10967,7 +10966,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="302" spans="1:5" hidden="1">
+    <row r="302" spans="1:5">
       <c r="A302" t="s">
         <v>1126</v>
       </c>
@@ -10984,7 +10983,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="303" spans="1:5" hidden="1">
+    <row r="303" spans="1:5">
       <c r="A303" t="s">
         <v>1130</v>
       </c>
@@ -11001,7 +11000,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="304" spans="1:5" hidden="1">
+    <row r="304" spans="1:5">
       <c r="A304" t="s">
         <v>1134</v>
       </c>
@@ -11035,7 +11034,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1">
+    <row r="306" spans="1:5">
       <c r="A306" t="s">
         <v>1142</v>
       </c>
@@ -11052,7 +11051,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1">
+    <row r="307" spans="1:5">
       <c r="A307" t="s">
         <v>1146</v>
       </c>
@@ -11063,7 +11062,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1">
+    <row r="308" spans="1:5">
       <c r="A308" t="s">
         <v>1149</v>
       </c>
@@ -11074,7 +11073,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1">
+    <row r="309" spans="1:5">
       <c r="A309" t="s">
         <v>1152</v>
       </c>
@@ -11085,7 +11084,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1">
+    <row r="310" spans="1:5">
       <c r="A310" t="s">
         <v>1155</v>
       </c>
@@ -11102,7 +11101,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1">
+    <row r="311" spans="1:5">
       <c r="A311" t="s">
         <v>1159</v>
       </c>
@@ -11119,7 +11118,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1">
+    <row r="312" spans="1:5">
       <c r="A312" t="s">
         <v>1163</v>
       </c>
@@ -11136,7 +11135,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1">
+    <row r="313" spans="1:5">
       <c r="A313" t="s">
         <v>1167</v>
       </c>
@@ -11153,7 +11152,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1">
+    <row r="314" spans="1:5">
       <c r="A314" t="s">
         <v>1171</v>
       </c>
@@ -11170,7 +11169,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1">
+    <row r="315" spans="1:5">
       <c r="A315" t="s">
         <v>1175</v>
       </c>
@@ -11187,7 +11186,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1">
+    <row r="316" spans="1:5">
       <c r="A316" t="s">
         <v>1179</v>
       </c>
@@ -11204,7 +11203,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1">
+    <row r="317" spans="1:5">
       <c r="A317" t="s">
         <v>1183</v>
       </c>
@@ -11221,7 +11220,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1">
+    <row r="318" spans="1:5">
       <c r="A318" t="s">
         <v>1187</v>
       </c>
@@ -11249,7 +11248,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1">
+    <row r="320" spans="1:5">
       <c r="A320" t="s">
         <v>1194</v>
       </c>
@@ -11260,7 +11259,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1">
+    <row r="321" spans="1:5">
       <c r="A321" t="s">
         <v>1197</v>
       </c>
@@ -11277,7 +11276,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1">
+    <row r="322" spans="1:5">
       <c r="A322" t="s">
         <v>1201</v>
       </c>
@@ -11288,7 +11287,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1">
+    <row r="323" spans="1:5">
       <c r="A323" t="s">
         <v>1204</v>
       </c>
@@ -11305,7 +11304,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1">
+    <row r="324" spans="1:5">
       <c r="A324" t="s">
         <v>1208</v>
       </c>
@@ -11316,7 +11315,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="325" spans="1:5" hidden="1">
+    <row r="325" spans="1:5">
       <c r="A325" t="s">
         <v>1211</v>
       </c>
@@ -11333,7 +11332,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="326" spans="1:5" hidden="1">
+    <row r="326" spans="1:5">
       <c r="A326" t="s">
         <v>1215</v>
       </c>
@@ -11344,7 +11343,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="327" spans="1:5" ht="30" hidden="1">
+    <row r="327" spans="1:5" ht="30">
       <c r="A327" t="s">
         <v>1218</v>
       </c>
@@ -11361,7 +11360,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="328" spans="1:5" hidden="1">
+    <row r="328" spans="1:5">
       <c r="A328" t="s">
         <v>1222</v>
       </c>
@@ -11378,7 +11377,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1">
+    <row r="329" spans="1:5">
       <c r="A329" t="s">
         <v>1226</v>
       </c>
@@ -11389,7 +11388,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="330" spans="1:5" hidden="1">
+    <row r="330" spans="1:5">
       <c r="A330" t="s">
         <v>1229</v>
       </c>
@@ -11406,7 +11405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="331" spans="1:5" hidden="1">
+    <row r="331" spans="1:5">
       <c r="A331" t="s">
         <v>1233</v>
       </c>
@@ -11423,7 +11422,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="332" spans="1:5" hidden="1">
+    <row r="332" spans="1:5">
       <c r="A332" t="s">
         <v>1237</v>
       </c>
@@ -11457,7 +11456,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="334" spans="1:5" hidden="1">
+    <row r="334" spans="1:5">
       <c r="A334" t="s">
         <v>1245</v>
       </c>
@@ -11491,7 +11490,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="336" spans="1:5" hidden="1">
+    <row r="336" spans="1:5">
       <c r="A336" t="s">
         <v>1253</v>
       </c>
@@ -11502,7 +11501,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="337" spans="1:5" hidden="1">
+    <row r="337" spans="1:5">
       <c r="A337" t="s">
         <v>1256</v>
       </c>
@@ -11513,7 +11512,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="338" spans="1:5" hidden="1">
+    <row r="338" spans="1:5">
       <c r="A338" t="s">
         <v>1259</v>
       </c>
@@ -11530,7 +11529,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="339" spans="1:5" hidden="1">
+    <row r="339" spans="1:5">
       <c r="A339" t="s">
         <v>1263</v>
       </c>
@@ -11547,7 +11546,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="340" spans="1:5" hidden="1">
+    <row r="340" spans="1:5">
       <c r="A340" t="s">
         <v>1267</v>
       </c>
@@ -11558,7 +11557,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="341" spans="1:5" hidden="1">
+    <row r="341" spans="1:5">
       <c r="A341" t="s">
         <v>1270</v>
       </c>
@@ -11575,7 +11574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="342" spans="1:5" hidden="1">
+    <row r="342" spans="1:5">
       <c r="A342" t="s">
         <v>1274</v>
       </c>
@@ -11592,7 +11591,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="343" spans="1:5" hidden="1">
+    <row r="343" spans="1:5">
       <c r="A343" t="s">
         <v>1278</v>
       </c>
@@ -11609,7 +11608,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="344" spans="1:5" hidden="1">
+    <row r="344" spans="1:5">
       <c r="A344" t="s">
         <v>1282</v>
       </c>
@@ -11626,7 +11625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="345" spans="1:5" hidden="1">
+    <row r="345" spans="1:5">
       <c r="A345" t="s">
         <v>1286</v>
       </c>
@@ -11643,7 +11642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="346" spans="1:5" hidden="1">
+    <row r="346" spans="1:5">
       <c r="A346" t="s">
         <v>1290</v>
       </c>
@@ -11654,7 +11653,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="347" spans="1:5" hidden="1">
+    <row r="347" spans="1:5">
       <c r="A347" t="s">
         <v>1293</v>
       </c>
@@ -11671,7 +11670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="348" spans="1:5" hidden="1">
+    <row r="348" spans="1:5">
       <c r="A348" t="s">
         <v>1297</v>
       </c>
@@ -11688,7 +11687,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="349" spans="1:5" hidden="1">
+    <row r="349" spans="1:5">
       <c r="A349" t="s">
         <v>1301</v>
       </c>
@@ -11705,7 +11704,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="350" spans="1:5" hidden="1">
+    <row r="350" spans="1:5">
       <c r="A350" t="s">
         <v>1305</v>
       </c>
@@ -11722,7 +11721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="351" spans="1:5" hidden="1">
+    <row r="351" spans="1:5">
       <c r="A351" t="s">
         <v>1309</v>
       </c>
@@ -11739,7 +11738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="352" spans="1:5" hidden="1">
+    <row r="352" spans="1:5">
       <c r="A352" t="s">
         <v>1313</v>
       </c>
@@ -11750,7 +11749,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="353" spans="1:5" hidden="1">
+    <row r="353" spans="1:5">
       <c r="A353" t="s">
         <v>1316</v>
       </c>
@@ -11767,7 +11766,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="354" spans="1:5" hidden="1">
+    <row r="354" spans="1:5">
       <c r="A354" t="s">
         <v>1320</v>
       </c>
@@ -11778,7 +11777,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="355" spans="1:5" hidden="1">
+    <row r="355" spans="1:5">
       <c r="A355" t="s">
         <v>1323</v>
       </c>
@@ -11789,7 +11788,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="356" spans="1:5" hidden="1">
+    <row r="356" spans="1:5">
       <c r="A356" t="s">
         <v>1326</v>
       </c>
@@ -11806,7 +11805,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="357" spans="1:5" hidden="1">
+    <row r="357" spans="1:5">
       <c r="A357" t="s">
         <v>1330</v>
       </c>
@@ -11823,7 +11822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="358" spans="1:5" hidden="1">
+    <row r="358" spans="1:5">
       <c r="A358" t="s">
         <v>1334</v>
       </c>
@@ -11840,7 +11839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="359" spans="1:5" hidden="1">
+    <row r="359" spans="1:5">
       <c r="A359" t="s">
         <v>1338</v>
       </c>
@@ -11857,7 +11856,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="360" spans="1:5" hidden="1">
+    <row r="360" spans="1:5">
       <c r="A360" t="s">
         <v>1342</v>
       </c>
@@ -11874,7 +11873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="361" spans="1:5" hidden="1">
+    <row r="361" spans="1:5">
       <c r="A361" t="s">
         <v>1346</v>
       </c>
@@ -11885,7 +11884,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="362" spans="1:5" hidden="1">
+    <row r="362" spans="1:5">
       <c r="A362" t="s">
         <v>1349</v>
       </c>
@@ -11896,7 +11895,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="363" spans="1:5" hidden="1">
+    <row r="363" spans="1:5">
       <c r="A363" t="s">
         <v>1352</v>
       </c>
@@ -11913,7 +11912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="364" spans="1:5" hidden="1">
+    <row r="364" spans="1:5">
       <c r="A364" t="s">
         <v>1356</v>
       </c>
@@ -11924,7 +11923,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="365" spans="1:5" hidden="1">
+    <row r="365" spans="1:5">
       <c r="A365" t="s">
         <v>1359</v>
       </c>
@@ -11935,7 +11934,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="366" spans="1:5" hidden="1">
+    <row r="366" spans="1:5">
       <c r="A366" t="s">
         <v>1362</v>
       </c>
@@ -11952,7 +11951,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="367" spans="1:5" hidden="1">
+    <row r="367" spans="1:5">
       <c r="A367" t="s">
         <v>1366</v>
       </c>
@@ -11969,7 +11968,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="368" spans="1:5" hidden="1">
+    <row r="368" spans="1:5">
       <c r="A368" t="s">
         <v>1370</v>
       </c>
@@ -11986,7 +11985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="369" spans="1:5" hidden="1">
+    <row r="369" spans="1:5">
       <c r="A369" t="s">
         <v>1374</v>
       </c>
@@ -12003,7 +12002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="370" spans="1:5" ht="30" hidden="1">
+    <row r="370" spans="1:5" ht="30">
       <c r="A370" t="s">
         <v>1378</v>
       </c>
@@ -12020,7 +12019,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="371" spans="1:5" hidden="1">
+    <row r="371" spans="1:5">
       <c r="A371" t="s">
         <v>1382</v>
       </c>
@@ -12037,7 +12036,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="372" spans="1:5" hidden="1">
+    <row r="372" spans="1:5">
       <c r="A372" t="s">
         <v>1386</v>
       </c>
@@ -12054,7 +12053,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="373" spans="1:5" hidden="1">
+    <row r="373" spans="1:5">
       <c r="A373" t="s">
         <v>1390</v>
       </c>
@@ -12071,7 +12070,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="374" spans="1:5" hidden="1">
+    <row r="374" spans="1:5">
       <c r="A374" t="s">
         <v>1394</v>
       </c>
@@ -12088,7 +12087,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="375" spans="1:5" hidden="1">
+    <row r="375" spans="1:5">
       <c r="A375" t="s">
         <v>1398</v>
       </c>
@@ -12105,7 +12104,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="376" spans="1:5" hidden="1">
+    <row r="376" spans="1:5">
       <c r="A376" t="s">
         <v>1402</v>
       </c>
@@ -12122,7 +12121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="377" spans="1:5" hidden="1">
+    <row r="377" spans="1:5">
       <c r="A377" t="s">
         <v>1406</v>
       </c>
@@ -12139,7 +12138,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="378" spans="1:5" hidden="1">
+    <row r="378" spans="1:5">
       <c r="A378" t="s">
         <v>1410</v>
       </c>
@@ -12156,7 +12155,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="379" spans="1:5" hidden="1">
+    <row r="379" spans="1:5">
       <c r="A379" t="s">
         <v>1414</v>
       </c>
@@ -12167,7 +12166,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="380" spans="1:5" hidden="1">
+    <row r="380" spans="1:5">
       <c r="A380" t="s">
         <v>1417</v>
       </c>
@@ -12184,7 +12183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="381" spans="1:5" hidden="1">
+    <row r="381" spans="1:5">
       <c r="A381" t="s">
         <v>1421</v>
       </c>
@@ -12195,7 +12194,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="382" spans="1:5" hidden="1">
+    <row r="382" spans="1:5">
       <c r="A382" t="s">
         <v>1424</v>
       </c>
@@ -12212,7 +12211,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="383" spans="1:5" hidden="1">
+    <row r="383" spans="1:5">
       <c r="A383" t="s">
         <v>1428</v>
       </c>
@@ -12229,7 +12228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="384" spans="1:5" hidden="1">
+    <row r="384" spans="1:5">
       <c r="A384" t="s">
         <v>1432</v>
       </c>
@@ -12246,7 +12245,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="385" spans="1:5" hidden="1">
+    <row r="385" spans="1:5">
       <c r="A385" t="s">
         <v>1436</v>
       </c>
@@ -12263,7 +12262,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="386" spans="1:5" hidden="1">
+    <row r="386" spans="1:5">
       <c r="A386" t="s">
         <v>1440</v>
       </c>
@@ -12274,7 +12273,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="387" spans="1:5" hidden="1">
+    <row r="387" spans="1:5">
       <c r="A387" t="s">
         <v>1443</v>
       </c>
@@ -12291,7 +12290,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="388" spans="1:5" hidden="1">
+    <row r="388" spans="1:5">
       <c r="A388" t="s">
         <v>1447</v>
       </c>
@@ -12325,7 +12324,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="390" spans="1:5" hidden="1">
+    <row r="390" spans="1:5">
       <c r="A390" t="s">
         <v>1455</v>
       </c>
@@ -12342,7 +12341,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="391" spans="1:5" hidden="1">
+    <row r="391" spans="1:5">
       <c r="A391" t="s">
         <v>1459</v>
       </c>
@@ -12359,7 +12358,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="392" spans="1:5" hidden="1">
+    <row r="392" spans="1:5">
       <c r="A392" t="s">
         <v>1463</v>
       </c>
@@ -12376,7 +12375,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="393" spans="1:5" hidden="1">
+    <row r="393" spans="1:5">
       <c r="A393" t="s">
         <v>1467</v>
       </c>
@@ -12393,7 +12392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="394" spans="1:5" hidden="1">
+    <row r="394" spans="1:5">
       <c r="A394" t="s">
         <v>1471</v>
       </c>
@@ -12410,7 +12409,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="395" spans="1:5" hidden="1">
+    <row r="395" spans="1:5">
       <c r="A395" t="s">
         <v>1475</v>
       </c>
@@ -12421,7 +12420,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="396" spans="1:5" hidden="1">
+    <row r="396" spans="1:5">
       <c r="A396" t="s">
         <v>1478</v>
       </c>
@@ -12438,7 +12437,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="397" spans="1:5" hidden="1">
+    <row r="397" spans="1:5">
       <c r="A397" t="s">
         <v>1482</v>
       </c>
@@ -12455,7 +12454,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="398" spans="1:5" hidden="1">
+    <row r="398" spans="1:5">
       <c r="A398" t="s">
         <v>1486</v>
       </c>
@@ -12472,7 +12471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="399" spans="1:5" hidden="1">
+    <row r="399" spans="1:5">
       <c r="A399" t="s">
         <v>1490</v>
       </c>
@@ -12483,7 +12482,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="400" spans="1:5" hidden="1">
+    <row r="400" spans="1:5">
       <c r="A400" t="s">
         <v>1493</v>
       </c>
@@ -12500,7 +12499,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="401" spans="1:5" hidden="1">
+    <row r="401" spans="1:5">
       <c r="A401" t="s">
         <v>1497</v>
       </c>
@@ -12511,7 +12510,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="402" spans="1:5" hidden="1">
+    <row r="402" spans="1:5">
       <c r="A402" t="s">
         <v>1500</v>
       </c>
@@ -12528,7 +12527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="403" spans="1:5" hidden="1">
+    <row r="403" spans="1:5">
       <c r="A403" t="s">
         <v>1504</v>
       </c>
@@ -12539,7 +12538,7 @@
         <v>1506</v>
       </c>
     </row>
-    <row r="404" spans="1:5" hidden="1">
+    <row r="404" spans="1:5">
       <c r="A404" t="s">
         <v>1507</v>
       </c>
@@ -12556,7 +12555,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="405" spans="1:5" hidden="1">
+    <row r="405" spans="1:5">
       <c r="A405" t="s">
         <v>1511</v>
       </c>
@@ -12567,7 +12566,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="406" spans="1:5" hidden="1">
+    <row r="406" spans="1:5">
       <c r="A406" t="s">
         <v>1514</v>
       </c>
@@ -12584,7 +12583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="407" spans="1:5" hidden="1">
+    <row r="407" spans="1:5">
       <c r="A407" t="s">
         <v>1518</v>
       </c>
@@ -12595,7 +12594,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="408" spans="1:5" hidden="1">
+    <row r="408" spans="1:5">
       <c r="A408" t="s">
         <v>1521</v>
       </c>
@@ -12612,7 +12611,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="409" spans="1:5" hidden="1">
+    <row r="409" spans="1:5">
       <c r="A409" t="s">
         <v>1525</v>
       </c>
@@ -12629,7 +12628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="410" spans="1:5" ht="30" hidden="1">
+    <row r="410" spans="1:5" ht="30">
       <c r="A410" t="s">
         <v>1529</v>
       </c>
@@ -12647,14 +12646,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E410" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="AI_x000a_"/>
-        <filter val="Al"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="E1:E410" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>